<commit_message>
fix bug import + search + file data
</commit_message>
<xml_diff>
--- a/ProjectMyShop/phonedata.xlsx
+++ b/ProjectMyShop/phonedata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021-2022 Semester II\Windows Programming\InClass\Binding_Converter_19127646\Binding_Converter_19127646\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DD9A32-EBCF-4599-862B-A094A7C271F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD9CBF1-58CC-4D45-8FEE-96BCB6F56675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iPhone" sheetId="1" r:id="rId1"/>
@@ -179,96 +179,6 @@
     <t>Xiaomi</t>
   </si>
   <si>
-    <t>Images/iphone/avatar01.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar02.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar03.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar04.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar05.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar06.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar07.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar08.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar09.jpg</t>
-  </si>
-  <si>
-    <t>Images/iphone/avatar10.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar01.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar02.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar03.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar04.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar05.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar06.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar07.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar08.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar09.jpg</t>
-  </si>
-  <si>
-    <t>Images/samsung/avatar10.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar02.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar03.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar04.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar05.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar06.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar07.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar08.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar09.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar10.jpg</t>
-  </si>
-  <si>
-    <t>Images/xiaomi/avatar01.jpg</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
@@ -276,6 +186,96 @@
   </si>
   <si>
     <t>UploadDate</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar02.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar03.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar04.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar05.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar06.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar07.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar08.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar09.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar10.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\iphone\avatar01.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar02.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar01.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar03.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar04.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar05.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar06.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar07.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar08.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar09.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\samsung\avatar10.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar01.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar02.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar03.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar04.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar05.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar06.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar07.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar08.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar09.jpg</t>
+  </si>
+  <si>
+    <t>D:\Images\xiaomi\avatar10.jpg</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="B3:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I17"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,13 +631,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="J3" t="s">
         <v>8</v>
@@ -665,7 +665,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -690,7 +690,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -740,7 +740,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -765,7 +765,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -790,7 +790,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -840,7 +840,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -890,7 +890,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -915,7 +915,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
@@ -965,7 +965,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06006F5-7BD8-4D8D-A61A-910BD5261FBD}">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,13 +1031,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>8</v>
@@ -1065,7 +1065,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -1090,7 +1090,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -1115,7 +1115,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -1140,7 +1140,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -1165,7 +1165,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -1190,7 +1190,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -1215,7 +1215,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -1240,7 +1240,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -1265,7 +1265,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -1315,7 +1315,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -1340,7 +1340,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
@@ -1365,7 +1365,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
@@ -1390,7 +1390,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76C9E61-3D4C-47E3-A2E4-C18C63FDF12B}">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,13 +1431,13 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>8</v>
@@ -1463,7 +1463,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -1486,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -1509,7 +1509,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -1532,7 +1532,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -1555,7 +1555,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -1578,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -1601,7 +1601,7 @@
         <v>7</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
         <v>9</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -1670,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -1693,7 +1693,7 @@
         <v>5</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -1716,7 +1716,7 @@
         <v>6</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
@@ -1739,7 +1739,7 @@
         <v>7</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
@@ -1762,7 +1762,7 @@
         <v>9</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>